<commit_message>
update des insert et update
</commit_message>
<xml_diff>
--- a/Fichiers modifiables/DonnéesExcel/update_parents.xlsx
+++ b/Fichiers modifiables/DonnéesExcel/update_parents.xlsx
@@ -352,8 +352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,11 +747,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>137</v>
-      </c>
-    </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>138</v>

</xml_diff>